<commit_message>
Made dots follow curved and rigid paths.
</commit_message>
<xml_diff>
--- a/Gloria Flux Order.xlsx
+++ b/Gloria Flux Order.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gloriahernandez/Desktop/GitHub/Carbon_Animation/Carbon_Pathway_Animation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{462C27E9-FE7D-0D42-BE5B-4F5225F1BA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1F9FF1-F922-0A40-9B2E-A0BCE598B0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{AEF66DF4-CE00-2F41-A546-DBAD6B391D62}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{AEF66DF4-CE00-2F41-A546-DBAD6B391D62}"/>
   </bookViews>
   <sheets>
     <sheet name="Order without Unnecessary Rxns" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="68">
   <si>
     <t>Group</t>
   </si>
@@ -237,13 +237,16 @@
   </si>
   <si>
     <t>Reaction ID</t>
+  </si>
+  <si>
+    <t>THIS ONE IS REPEATED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -251,13 +254,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -272,8 +292,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47F27B2-83C8-AE4F-ABC7-920D9438AF2C}">
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="142" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="142" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -690,7 +713,7 @@
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>63</v>
       </c>
     </row>
@@ -766,7 +789,7 @@
       <c r="C9">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E9" t="s">
@@ -811,7 +834,7 @@
       <c r="C12">
         <v>11</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>59</v>
       </c>
       <c r="E12" t="s">
@@ -870,7 +893,7 @@
       <c r="C16">
         <v>15</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1115,9 +1138,10 @@
       <c r="C32">
         <v>31</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
@@ -1132,7 +1156,7 @@
       <c r="D33" t="s">
         <v>51</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1191,7 +1215,7 @@
       <c r="D37" t="s">
         <v>56</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1367,7 +1391,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>16</v>
       </c>
@@ -1384,7 +1408,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>16</v>
       </c>
@@ -1398,7 +1422,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>17</v>
       </c>
@@ -1412,7 +1436,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>18</v>
       </c>
@@ -1429,7 +1453,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1</v>
       </c>
@@ -1443,7 +1467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2</v>
       </c>
@@ -1460,7 +1484,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2</v>
       </c>
@@ -1477,7 +1501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2</v>
       </c>
@@ -1494,7 +1518,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2</v>
       </c>
@@ -1508,7 +1532,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>3</v>
       </c>
@@ -1521,11 +1545,11 @@
       <c r="D58" t="s">
         <v>56</v>
       </c>
-      <c r="E58" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E58" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>3</v>
       </c>
@@ -1538,8 +1562,9 @@
       <c r="D59" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>4</v>
       </c>
@@ -1552,8 +1577,11 @@
       <c r="D60" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>5</v>
       </c>
@@ -1566,8 +1594,11 @@
       <c r="D61" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>6</v>
       </c>
@@ -1580,8 +1611,11 @@
       <c r="D62" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>6</v>
       </c>
@@ -1594,8 +1628,11 @@
       <c r="D63" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>7</v>
       </c>
@@ -1608,8 +1645,11 @@
       <c r="D64" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>7</v>
       </c>
@@ -1622,8 +1662,11 @@
       <c r="D65" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>7</v>
       </c>
@@ -1636,8 +1679,11 @@
       <c r="D66" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>7</v>
       </c>
@@ -1653,8 +1699,11 @@
       <c r="E67" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>8</v>
       </c>
@@ -1670,8 +1719,11 @@
       <c r="E68" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>8</v>
       </c>
@@ -1687,8 +1739,11 @@
       <c r="E69" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>8</v>
       </c>
@@ -1701,8 +1756,11 @@
       <c r="D70" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>8</v>
       </c>
@@ -1718,8 +1776,11 @@
       <c r="E71" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>8</v>
       </c>
@@ -1735,8 +1796,11 @@
       <c r="E72" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>8</v>
       </c>
@@ -1749,8 +1813,11 @@
       <c r="D73" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>8</v>
       </c>
@@ -1763,8 +1830,11 @@
       <c r="D74" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>8</v>
       </c>
@@ -1780,8 +1850,11 @@
       <c r="E75" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>8</v>
       </c>
@@ -1797,8 +1870,11 @@
       <c r="E76" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>9</v>
       </c>
@@ -1811,8 +1887,11 @@
       <c r="D77" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>9</v>
       </c>
@@ -1825,8 +1904,11 @@
       <c r="D78" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>9</v>
       </c>
@@ -1842,8 +1924,11 @@
       <c r="E79" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F79" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>9</v>
       </c>
@@ -1856,8 +1941,11 @@
       <c r="D80" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>9</v>
       </c>
@@ -1870,8 +1958,11 @@
       <c r="D81" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F81" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>9</v>
       </c>
@@ -1887,8 +1978,11 @@
       <c r="E82" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>9</v>
       </c>
@@ -1904,8 +1998,11 @@
       <c r="E83" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>10</v>
       </c>
@@ -1921,8 +2018,11 @@
       <c r="E84" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F84" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>10</v>
       </c>
@@ -1938,8 +2038,11 @@
       <c r="E85" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F85" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>10</v>
       </c>
@@ -1952,8 +2055,11 @@
       <c r="D86" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F86" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>10</v>
       </c>
@@ -1966,8 +2072,11 @@
       <c r="D87" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F87" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>10</v>
       </c>
@@ -1983,8 +2092,11 @@
       <c r="E88" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F88" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>11</v>
       </c>
@@ -2000,8 +2112,11 @@
       <c r="E89" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F89" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>11</v>
       </c>
@@ -2016,6 +2131,9 @@
       </c>
       <c r="E90" t="s">
         <v>64</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>